<commit_message>
Pretty big improvements to bitmap drawing code, and waterfall display code. Also a hack to deal with the red-things-stay-red bug (it's not ideal, it just blocks the encoder tick() if the display is drawing, doesn't seem to effect the feel of the interface in a bad way. Beginning to include GPS support. Working on some other display speedups (DMA and 16bit transfers, both are currently disabled)
</commit_message>
<xml_diff>
--- a/Documentation/Stepping through filter coeficient population.xlsx
+++ b/Documentation/Stepping through filter coeficient population.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7485"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14910" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5761,6 +5761,105 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="73964544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$1145:$G$1154</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.894348370484642E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14203952192020614</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27017522578732073</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42080777983773177</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57919222016226812</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.72982477421267922</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.85796047807979381</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95105651629515353</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="53992064"/>
+        <c:axId val="54055296"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="53992064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54055296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="54055296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="53992064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5836,6 +5935,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1146</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1160</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="Chart 16"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6129,10 +6258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S1138"/>
+  <dimension ref="A1:S1155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1107" workbookViewId="0">
-      <selection activeCell="E1146" sqref="E1146"/>
+    <sheetView tabSelected="1" topLeftCell="A1134" workbookViewId="0">
+      <selection activeCell="J1163" sqref="J1163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -48869,7 +48998,7 @@
         <v>-1.7194053729999999E-4</v>
       </c>
     </row>
-    <row r="1137" spans="2:11">
+    <row r="1137" spans="1:11">
       <c r="B1137" t="s">
         <v>99</v>
       </c>
@@ -48908,7 +49037,7 @@
         <v>2.305342934E-4</v>
       </c>
     </row>
-    <row r="1138" spans="2:11">
+    <row r="1138" spans="1:11">
       <c r="B1138" t="s">
         <v>100</v>
       </c>
@@ -48945,6 +49074,247 @@
       <c r="K1138">
         <f t="shared" si="61"/>
         <v>4.8343206470000003E-4</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:11">
+      <c r="C1145">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D1145">
+        <f>C1145/100*PI()</f>
+        <v>0</v>
+      </c>
+      <c r="E1145">
+        <f>SIN(D1145)</f>
+        <v>0</v>
+      </c>
+      <c r="F1145">
+        <f>E1145+F1144</f>
+        <v>0</v>
+      </c>
+      <c r="G1145">
+        <f>F1145/$F$1154</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:11">
+      <c r="A1146">
+        <v>10</v>
+      </c>
+      <c r="C1146">
+        <f>C1145+$A$1146</f>
+        <v>10</v>
+      </c>
+      <c r="D1146">
+        <f t="shared" ref="D1146:D1155" si="63">C1146/100*PI()</f>
+        <v>0.31415926535897931</v>
+      </c>
+      <c r="E1146">
+        <f t="shared" ref="E1146:E1155" si="64">SIN(D1146)</f>
+        <v>0.3090169943749474</v>
+      </c>
+      <c r="F1146">
+        <f t="shared" ref="F1146:F1155" si="65">E1146+F1145</f>
+        <v>0.3090169943749474</v>
+      </c>
+      <c r="G1146">
+        <f t="shared" ref="G1146:G1154" si="66">F1146/$F$1154</f>
+        <v>4.894348370484642E-2</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:11">
+      <c r="C1147">
+        <f t="shared" ref="C1147:C1168" si="67">C1146+$A$1146</f>
+        <v>20</v>
+      </c>
+      <c r="D1147">
+        <f t="shared" si="63"/>
+        <v>0.62831853071795862</v>
+      </c>
+      <c r="E1147">
+        <f t="shared" si="64"/>
+        <v>0.58778525229247314</v>
+      </c>
+      <c r="F1147">
+        <f t="shared" si="65"/>
+        <v>0.89680224666742059</v>
+      </c>
+      <c r="G1147">
+        <f t="shared" si="66"/>
+        <v>0.14203952192020614</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:11">
+      <c r="C1148">
+        <f t="shared" si="67"/>
+        <v>30</v>
+      </c>
+      <c r="D1148">
+        <f t="shared" si="63"/>
+        <v>0.94247779607693793</v>
+      </c>
+      <c r="E1148">
+        <f t="shared" si="64"/>
+        <v>0.80901699437494745</v>
+      </c>
+      <c r="F1148">
+        <f t="shared" si="65"/>
+        <v>1.705819241042368</v>
+      </c>
+      <c r="G1148">
+        <f t="shared" si="66"/>
+        <v>0.27017522578732073</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:11">
+      <c r="C1149">
+        <f t="shared" si="67"/>
+        <v>40</v>
+      </c>
+      <c r="D1149">
+        <f t="shared" si="63"/>
+        <v>1.2566370614359172</v>
+      </c>
+      <c r="E1149">
+        <f t="shared" si="64"/>
+        <v>0.95105651629515353</v>
+      </c>
+      <c r="F1149">
+        <f t="shared" si="65"/>
+        <v>2.6568757573375215</v>
+      </c>
+      <c r="G1149">
+        <f t="shared" si="66"/>
+        <v>0.42080777983773177</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:11">
+      <c r="C1150">
+        <f t="shared" si="67"/>
+        <v>50</v>
+      </c>
+      <c r="D1150">
+        <f t="shared" si="63"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="E1150">
+        <f t="shared" si="64"/>
+        <v>1</v>
+      </c>
+      <c r="F1150">
+        <f t="shared" si="65"/>
+        <v>3.6568757573375215</v>
+      </c>
+      <c r="G1150">
+        <f t="shared" si="66"/>
+        <v>0.57919222016226812</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:11">
+      <c r="C1151">
+        <f t="shared" si="67"/>
+        <v>60</v>
+      </c>
+      <c r="D1151">
+        <f t="shared" si="63"/>
+        <v>1.8849555921538759</v>
+      </c>
+      <c r="E1151">
+        <f t="shared" si="64"/>
+        <v>0.95105651629515364</v>
+      </c>
+      <c r="F1151">
+        <f t="shared" si="65"/>
+        <v>4.6079322736326755</v>
+      </c>
+      <c r="G1151">
+        <f t="shared" si="66"/>
+        <v>0.72982477421267922</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:11">
+      <c r="C1152">
+        <f t="shared" si="67"/>
+        <v>70</v>
+      </c>
+      <c r="D1152">
+        <f t="shared" si="63"/>
+        <v>2.1991148575128552</v>
+      </c>
+      <c r="E1152">
+        <f t="shared" si="64"/>
+        <v>0.80901699437494745</v>
+      </c>
+      <c r="F1152">
+        <f t="shared" si="65"/>
+        <v>5.416949268007623</v>
+      </c>
+      <c r="G1152">
+        <f t="shared" si="66"/>
+        <v>0.85796047807979381</v>
+      </c>
+    </row>
+    <row r="1153" spans="3:7">
+      <c r="C1153">
+        <f t="shared" si="67"/>
+        <v>80</v>
+      </c>
+      <c r="D1153">
+        <f t="shared" si="63"/>
+        <v>2.5132741228718345</v>
+      </c>
+      <c r="E1153">
+        <f t="shared" si="64"/>
+        <v>0.58778525229247325</v>
+      </c>
+      <c r="F1153">
+        <f t="shared" si="65"/>
+        <v>6.0047345203000964</v>
+      </c>
+      <c r="G1153">
+        <f t="shared" si="66"/>
+        <v>0.95105651629515353</v>
+      </c>
+    </row>
+    <row r="1154" spans="3:7">
+      <c r="C1154">
+        <f t="shared" si="67"/>
+        <v>90</v>
+      </c>
+      <c r="D1154">
+        <f t="shared" si="63"/>
+        <v>2.8274333882308138</v>
+      </c>
+      <c r="E1154">
+        <f t="shared" si="64"/>
+        <v>0.30901699437494751</v>
+      </c>
+      <c r="F1154">
+        <f t="shared" si="65"/>
+        <v>6.3137515146750438</v>
+      </c>
+      <c r="G1154">
+        <f t="shared" si="66"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1155" spans="3:7">
+      <c r="C1155">
+        <f t="shared" si="67"/>
+        <v>100</v>
+      </c>
+      <c r="D1155">
+        <f t="shared" si="63"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="E1155">
+        <f t="shared" si="64"/>
+        <v>1.22514845490862E-16</v>
+      </c>
+      <c r="F1155">
+        <f t="shared" si="65"/>
+        <v>6.3137515146750438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>